<commit_message>
Updated instructions and new buggy betas
</commit_message>
<xml_diff>
--- a/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
+++ b/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0571AD47-4914-A44D-BEC5-F13F02D9874A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EE4144-FDAE-4AD9-AC2E-CD0F1C7947C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="500" windowWidth="13060" windowHeight="14540" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="36288" yWindow="4860" windowWidth="17628" windowHeight="12024" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Criteria</t>
   </si>
@@ -84,7 +94,34 @@
     <t xml:space="preserve">   i/o in the HTML file</t>
   </si>
   <si>
-    <t xml:space="preserve">  Loop +  i/o oop in the HTML file</t>
+    <t xml:space="preserve">  Loop +  i/o  in the HTML file</t>
+  </si>
+  <si>
+    <t>Should have for loop</t>
+  </si>
+  <si>
+    <t>Validation with while loop</t>
+  </si>
+  <si>
+    <t>Repeat with do…while, validation with while</t>
+  </si>
+  <si>
+    <t>No if for alert</t>
+  </si>
+  <si>
+    <t>No if</t>
+  </si>
+  <si>
+    <t>Check num range, y/n</t>
+  </si>
+  <si>
+    <t>1) A. Countdown, B. Loan Repayment, C. Cycling Plan</t>
+  </si>
+  <si>
+    <t>2) A. Kindergarten Admit, B. Beverage Labeling,  C. Trail Difficulty Rating</t>
+  </si>
+  <si>
+    <t>3) A. Grade Level, B. State Tax, C. Trail Types</t>
   </si>
 </sst>
 </file>
@@ -141,11 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,15 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -506,10 +544,10 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="4">
         <v>10</v>
       </c>
     </row>
@@ -517,17 +555,17 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
         <v>2</v>
       </c>
     </row>
@@ -535,10 +573,10 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>4</v>
       </c>
     </row>
@@ -546,10 +584,10 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -557,10 +595,10 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>5</v>
       </c>
     </row>
@@ -568,10 +606,10 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>4</v>
       </c>
     </row>
@@ -579,10 +617,10 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>6</v>
       </c>
     </row>
@@ -590,10 +628,10 @@
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
         <v>2</v>
       </c>
     </row>
@@ -601,10 +639,10 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>6</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>6</v>
       </c>
     </row>
@@ -612,10 +650,10 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="4">
         <v>6</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="4">
         <v>6</v>
       </c>
     </row>
@@ -623,10 +661,10 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
         <v>2</v>
       </c>
     </row>
@@ -634,10 +672,10 @@
       <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
         <v>2</v>
       </c>
     </row>
@@ -654,8 +692,51 @@
         <v>50</v>
       </c>
     </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New practice problems and format change to rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
+++ b/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EE4144-FDAE-4AD9-AC2E-CD0F1C7947C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D6F02-0F82-5645-886D-BB04EBA40207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36288" yWindow="4860" windowWidth="17628" windowHeight="12024" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="10460" yWindow="1620" windowWidth="17620" windowHeight="14540" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Group A" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Score" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Criteria</t>
   </si>
@@ -122,13 +113,16 @@
   </si>
   <si>
     <t>3) A. Grade Level, B. State Tax, C. Trail Types</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +151,12 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,12 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,15 +499,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -529,9 +530,7 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
@@ -547,9 +546,7 @@
       <c r="D6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="4">
-        <v>10</v>
-      </c>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
@@ -565,9 +562,7 @@
       <c r="D8" s="4">
         <v>2</v>
       </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -576,9 +571,7 @@
       <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9" s="4">
-        <v>4</v>
-      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -587,9 +580,7 @@
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -598,9 +589,7 @@
       <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="4">
-        <v>5</v>
-      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -609,9 +598,7 @@
       <c r="D12" s="4">
         <v>4</v>
       </c>
-      <c r="E12" s="4">
-        <v>4</v>
-      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
@@ -620,9 +607,7 @@
       <c r="D13" s="4">
         <v>6</v>
       </c>
-      <c r="E13" s="4">
-        <v>6</v>
-      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -631,9 +616,7 @@
       <c r="D14" s="4">
         <v>2</v>
       </c>
-      <c r="E14" s="4">
-        <v>2</v>
-      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -642,11 +625,205 @@
       <c r="D15" s="4">
         <v>6</v>
       </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="4">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D6:D18)</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F217103E-3C1D-D743-A56A-64A1F3EA3BAA}">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6</v>
+      </c>
       <c r="E15" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
New and revised rubrics
</commit_message>
<xml_diff>
--- a/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
+++ b/Labs/Lab04/CS133JS_Lab04_Rubric.xlsx
@@ -1,36 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS133JS-CourseMaterials\Labs\Lab04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA08AD92-D159-428C-AB72-01F79DC4E94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA3316-69CB-C643-B50E-59F7F1D6AA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13068" yWindow="4968" windowWidth="17556" windowHeight="11592" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="-25200" yWindow="4280" windowWidth="23420" windowHeight="15720" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Score" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -515,13 +504,13 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C32"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.796875" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -579,7 +568,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -595,7 +584,7 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -603,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -611,7 +600,7 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -627,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -635,7 +624,7 @@
         <v>17</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -660,7 +649,7 @@
       </c>
       <c r="D20">
         <f>SUM(D6:D18)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -673,15 +662,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F217103E-3C1D-D743-A56A-64A1F3EA3BAA}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="18.19921875" customWidth="1"/>
-    <col min="4" max="4" width="7.796875" customWidth="1"/>
-    <col min="5" max="5" width="5.59765625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="1" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
@@ -757,10 +746,10 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -781,10 +770,10 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -793,10 +782,10 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -805,10 +794,10 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -829,10 +818,10 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -841,10 +830,10 @@
         <v>17</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -878,11 +867,11 @@
       </c>
       <c r="D20">
         <f>SUM(D6:D18)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <f>SUM(E6:E18)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7">

</xml_diff>